<commit_message>
Help And Support Feature
</commit_message>
<xml_diff>
--- a/Selenium-Scripts/src/HomeMoveTestData.xlsx
+++ b/Selenium-Scripts/src/HomeMoveTestData.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SetUp" sheetId="1" r:id="rId1"/>
     <sheet name="HomePage" sheetId="2" r:id="rId2"/>
     <sheet name="LoginPage" sheetId="3" r:id="rId3"/>
-    <sheet name="HelpAndSupport" sheetId="4" r:id="rId4"/>
+    <sheet name="HelpAndSupportPage" sheetId="4" r:id="rId4"/>
+    <sheet name="FeedBackPage" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>Key</t>
   </si>
@@ -90,10 +91,19 @@
     <t>tvsap199aa</t>
   </si>
   <si>
-    <t>searchQuery</t>
-  </si>
-  <si>
-    <t>Sim</t>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>faqText</t>
+  </si>
+  <si>
+    <t>Was your issue resolved?</t>
+  </si>
+  <si>
+    <t>feedBackText</t>
+  </si>
+  <si>
+    <t>This is the problem</t>
   </si>
 </sst>
 </file>
@@ -119,6 +129,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -498,17 +509,17 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -522,7 +533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -544,15 +555,16 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -560,7 +572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -568,7 +580,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -576,7 +588,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -584,7 +596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -592,7 +604,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -600,7 +612,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
@@ -618,16 +630,16 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -635,7 +647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -643,7 +655,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -658,19 +670,71 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -678,12 +742,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
         <v>23</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>